<commit_message>
hotel bug and template bug
</commit_message>
<xml_diff>
--- a/hotel-saas-frontend/public/user/file/property_price_template.xlsx
+++ b/hotel-saas-frontend/public/user/file/property_price_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\rankme Live\hotel-saas-frontend\public\user\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370F0F33-311B-4A4C-B804-25F3C8B191CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F01F7B3-949B-478F-9614-4AF3DC1FC47E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F091794C-8C41-4675-A5F2-35AF64A5BBE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>My Property</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Comp #5</t>
-  </si>
-  <si>
-    <t>nl</t>
   </si>
   <si>
     <t>My Propert Name</t>
@@ -201,11 +198,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,21 +225,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF121617"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FF121617"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color rgb="FF121617"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -270,24 +253,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -363,40 +334,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -737,7 +701,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -753,82 +717,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30.6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="3">
-        <v>45870</v>
-      </c>
-      <c r="B3" s="1">
-        <v>73</v>
-      </c>
-      <c r="C3" s="2">
-        <f>AVERAGE(D3:G3)</f>
-        <v>80.25</v>
-      </c>
-      <c r="D3" s="1">
-        <v>79</v>
-      </c>
-      <c r="E3" s="1">
-        <v>75</v>
-      </c>
-      <c r="F3" s="1">
-        <v>78</v>
-      </c>
-      <c r="G3" s="1">
-        <v>89</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
+    </row>
+    <row r="3" spans="1:8" ht="14.25" x14ac:dyDescent="0.45"/>
     <row r="4" spans="1:8" ht="14.25" x14ac:dyDescent="0.45"/>
     <row r="5" spans="1:8" ht="14.25" x14ac:dyDescent="0.45"/>
     <row r="6" spans="1:8" ht="14.25" x14ac:dyDescent="0.45"/>
@@ -852,231 +790,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.45">
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="4">
+      <c r="A3" s="1">
         <v>45870</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>0.16669999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
+      <c r="A4" s="1">
         <v>45871</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="3">
         <v>0.16669999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="4">
+      <c r="A5" s="1">
         <v>45872</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="3">
         <v>0.1852</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="4">
+      <c r="A6" s="1">
         <v>45873</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="3">
         <v>0.1852</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="4">
+      <c r="A7" s="1">
         <v>45874</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="3">
         <v>0.1852</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="4">
+      <c r="A8" s="1">
         <v>45875</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="3">
         <v>0.1111</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="4">
+      <c r="A9" s="1">
         <v>45876</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="3">
         <v>7.4099999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="4">
+      <c r="A10" s="1">
         <v>45877</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="3">
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="4">
+      <c r="A11" s="1">
         <v>45878</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="4">
+      <c r="A12" s="1">
         <v>45879</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="3">
         <v>0.1111</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="4">
+      <c r="A13" s="1">
         <v>45880</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="3">
         <v>0.14810000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="4">
+      <c r="A14" s="1">
         <v>45881</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="3">
         <v>9.2600000000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="4">
+      <c r="A15" s="1">
         <v>45882</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="4">
+      <c r="A16" s="1">
         <v>45883</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="4">
+      <c r="A17" s="1">
         <v>45884</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>1.8499999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="4">
+      <c r="A18" s="1">
         <v>45885</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="4">
+      <c r="A19" s="1">
         <v>45886</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="3">
         <v>0.1852</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="4">
+      <c r="A20" s="1">
         <v>45887</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="3">
         <v>0.16669999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="4">
+      <c r="A21" s="1">
         <v>45888</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="3">
         <v>0.2407</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="4">
+      <c r="A22" s="1">
         <v>45889</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="3">
         <v>0.1852</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="4">
+      <c r="A23" s="1">
         <v>45890</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="3">
         <v>9.2600000000000002E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="4">
+      <c r="A24" s="1">
         <v>45891</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="3">
         <v>0.38890000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="4">
+      <c r="A25" s="1">
         <v>45892</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="3">
         <v>0.38890000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="4">
+      <c r="A26" s="1">
         <v>45893</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="3">
         <v>1.8499999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="4">
+      <c r="A27" s="1">
         <v>45894</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="3">
         <v>7.4099999999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="4">
+      <c r="A28" s="1">
         <v>45895</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="3">
         <v>5.5599999999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="4">
+      <c r="A29" s="1">
         <v>45896</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1097,34 +1035,34 @@
   <cols>
     <col min="1" max="1" width="15.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" style="10" customWidth="1"/>
     <col min="5" max="5" width="14.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1132,17 +1070,17 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <v>0.64080000000000004</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>76.56</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <f>B3*C3</f>
         <v>49.059648000000003</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>4670</v>
       </c>
     </row>
@@ -1150,17 +1088,17 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>0.82520000000000004</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <v>68.239999999999995</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <f t="shared" ref="D4:D32" si="0">B4*C4</f>
         <v>56.311647999999998</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>5390.87</v>
       </c>
     </row>
@@ -1168,17 +1106,17 @@
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="2">
         <v>0.43809999999999999</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="10">
         <v>64.97</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <f t="shared" si="0"/>
         <v>28.463356999999998</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>2793.71</v>
       </c>
     </row>
@@ -1186,17 +1124,17 @@
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="2">
         <v>0.47060000000000002</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="10">
         <v>65.06</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <f t="shared" si="0"/>
         <v>30.617236000000002</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>2992.68</v>
       </c>
     </row>
@@ -1204,17 +1142,17 @@
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="2">
         <v>0.68930000000000002</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <v>63.24</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <f t="shared" si="0"/>
         <v>43.591332000000001</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>4426.8100000000004</v>
       </c>
     </row>
@@ -1222,17 +1160,17 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="2">
         <v>0.94679999999999997</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <v>88.57</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <f t="shared" si="0"/>
         <v>83.858075999999997</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>7262.47</v>
       </c>
     </row>
@@ -1240,17 +1178,17 @@
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="2">
         <v>0.85150000000000003</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="10">
         <v>90.05</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="10">
         <f t="shared" si="0"/>
         <v>76.677575000000004</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>7474.02</v>
       </c>
     </row>
@@ -1258,17 +1196,17 @@
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>0.74229999999999996</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="10">
         <v>71.459999999999994</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="10">
         <f t="shared" si="0"/>
         <v>53.044757999999995</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>4787.96</v>
       </c>
     </row>
@@ -1276,17 +1214,17 @@
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="2">
         <v>0.505</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="10">
         <v>71.52</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="10">
         <f t="shared" si="0"/>
         <v>36.117599999999996</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>3361.57</v>
       </c>
     </row>
@@ -1294,17 +1232,17 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>0.51429999999999998</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="10">
         <v>63.99</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <f t="shared" si="0"/>
         <v>32.910057000000002</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>3455.35</v>
       </c>
     </row>
@@ -1312,17 +1250,17 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="2">
         <v>0.63729999999999998</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="10">
         <v>71.61</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <f t="shared" si="0"/>
         <v>45.637052999999995</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="4">
         <v>4368.5</v>
       </c>
     </row>
@@ -1330,17 +1268,17 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>0.70299999999999996</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="10">
         <v>68.19</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <f t="shared" si="0"/>
         <v>47.937569999999994</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>4773.49</v>
       </c>
     </row>
@@ -1348,17 +1286,17 @@
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>0.96699999999999997</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>93.65</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="10">
         <f t="shared" si="0"/>
         <v>90.559550000000002</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>7773.31</v>
       </c>
     </row>
@@ -1366,17 +1304,17 @@
       <c r="A16" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>1.0112000000000001</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="10">
         <v>94.87</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="10">
         <f t="shared" si="0"/>
         <v>95.932544000000007</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>8158.57</v>
       </c>
     </row>
@@ -1384,17 +1322,17 @@
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="2">
         <v>0.9032</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="10">
         <v>66.180000000000007</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="10">
         <f t="shared" si="0"/>
         <v>59.773776000000005</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>5294.1</v>
       </c>
     </row>
@@ -1402,17 +1340,17 @@
       <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="2">
         <v>0.7228</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="10">
         <v>55.97</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="10">
         <f t="shared" si="0"/>
         <v>40.455115999999997</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>3862.07</v>
       </c>
     </row>
@@ -1420,17 +1358,17 @@
       <c r="A19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="2">
         <v>0.71289999999999998</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C19" s="10">
         <v>63.28</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19" s="10">
         <f t="shared" si="0"/>
         <v>45.112312000000003</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>4429.26</v>
       </c>
     </row>
@@ -1438,17 +1376,17 @@
       <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="2">
         <v>0.82179999999999997</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C20" s="10">
         <v>61.21</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20" s="10">
         <f t="shared" si="0"/>
         <v>50.302377999999997</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>5019.42</v>
       </c>
     </row>
@@ -1456,17 +1394,17 @@
       <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="2">
         <v>0.95150000000000001</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C21" s="10">
         <v>70.12</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="10">
         <f t="shared" si="0"/>
         <v>66.719180000000009</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>6591.72</v>
       </c>
     </row>
@@ -1474,17 +1412,17 @@
       <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="2">
         <v>1.0396000000000001</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="10">
         <v>96.07</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="10">
         <f t="shared" si="0"/>
         <v>99.874371999999994</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>9703.26</v>
       </c>
     </row>
@@ -1492,17 +1430,17 @@
       <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="2">
         <v>1</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C23" s="10">
         <v>92.43</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="10">
         <f t="shared" si="0"/>
         <v>92.43</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4">
         <v>9335.7999999999993</v>
       </c>
     </row>
@@ -1510,17 +1448,17 @@
       <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="2">
         <v>0.9899</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="10">
         <v>64.86</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="10">
         <f t="shared" si="0"/>
         <v>64.204914000000002</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="4">
         <v>6226.84</v>
       </c>
     </row>
@@ -1528,17 +1466,17 @@
       <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="2">
         <v>0.76239999999999997</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C25" s="10">
         <v>63.99</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="10">
         <f t="shared" si="0"/>
         <v>48.785975999999998</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>4671.42</v>
       </c>
     </row>
@@ -1546,17 +1484,17 @@
       <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="2">
         <v>0.66669999999999996</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="10">
         <v>64.86</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="10">
         <f t="shared" si="0"/>
         <v>43.242162</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="4">
         <v>4151.03</v>
       </c>
     </row>
@@ -1564,17 +1502,17 @@
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="2">
         <v>0.59409999999999996</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C27" s="10">
         <v>64.319999999999993</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27" s="10">
         <f t="shared" si="0"/>
         <v>38.212511999999997</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="4">
         <v>3794.74</v>
       </c>
     </row>
@@ -1582,17 +1520,17 @@
       <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="2">
         <v>0.63639999999999997</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C28" s="10">
         <v>70.02</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28" s="10">
         <f t="shared" si="0"/>
         <v>44.560727999999997</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>4060.93</v>
       </c>
     </row>
@@ -1600,17 +1538,17 @@
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="2">
         <v>0.7157</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C29" s="10">
         <v>93.58</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29" s="10">
         <f t="shared" si="0"/>
         <v>66.975206</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="4">
         <v>6082.9</v>
       </c>
     </row>
@@ -1618,17 +1556,17 @@
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="2">
         <v>0.91300000000000003</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="10">
         <v>94.18</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30" s="10">
         <f t="shared" si="0"/>
         <v>85.986340000000013</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>7440.29</v>
       </c>
     </row>
@@ -1636,17 +1574,17 @@
       <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="2">
         <v>0.70530000000000004</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C31" s="10">
         <v>72.64</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="10">
         <f t="shared" si="0"/>
         <v>51.232992000000003</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="4">
         <v>4576.03</v>
       </c>
     </row>
@@ -1654,17 +1592,17 @@
       <c r="A32" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="2">
         <v>0.70650000000000002</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C32" s="10">
         <v>70.39</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32" s="10">
         <f t="shared" si="0"/>
         <v>49.730535000000003</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="4">
         <v>4152.92</v>
       </c>
     </row>

</xml_diff>